<commit_message>
Update latex template to book format
MIgrated images to 144dpi png

Setup .gitignore
</commit_message>
<xml_diff>
--- a/docs/csv/configreg.xlsx
+++ b/docs/csv/configreg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="3300" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,19 +43,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
     </font>
     <font>
       <sz val="10"/>
@@ -85,6 +79,16 @@
       <color theme="1"/>
       <name val="Courier New"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,52 +183,65 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -234,6 +251,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -243,6 +262,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -575,7 +596,7 @@
   <dimension ref="B1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="A1:O3"/>
+      <selection activeCell="B2" sqref="B2:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -597,65 +618,65 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="10">
         <v>63</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10">
         <v>49</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="10">
         <v>48</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="10">
         <v>47</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10">
         <v>32</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="10">
         <v>31</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1">
+      <c r="K2" s="10"/>
+      <c r="L2" s="10">
         <v>16</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="10">
         <v>15</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1">
+      <c r="N2" s="10"/>
+      <c r="O2" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="21" thickBot="1">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="7">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="3" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="3" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="5"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
MIgrated images to 144dpi png
</commit_message>
<xml_diff>
--- a/docs/csv/configreg.xlsx
+++ b/docs/csv/configreg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="3300" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,19 +43,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
     </font>
     <font>
       <sz val="10"/>
@@ -85,6 +79,16 @@
       <color theme="1"/>
       <name val="Courier New"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,52 +183,65 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -234,6 +251,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -243,6 +262,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -575,7 +596,7 @@
   <dimension ref="B1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="A1:O3"/>
+      <selection activeCell="B2" sqref="B2:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -597,65 +618,65 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="10">
         <v>63</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10">
         <v>49</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="10">
         <v>48</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="10">
         <v>47</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10">
         <v>32</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="10">
         <v>31</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1">
+      <c r="K2" s="10"/>
+      <c r="L2" s="10">
         <v>16</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="10">
         <v>15</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1">
+      <c r="N2" s="10"/>
+      <c r="O2" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="21" thickBot="1">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="7">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="3" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="3" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="5"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>